<commit_message>
Feito várias alterações e ajustes no projeto.
</commit_message>
<xml_diff>
--- a/banco_de_dados/clientes.xlsx
+++ b/banco_de_dados/clientes.xlsx
@@ -58,13 +58,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
@@ -437,7 +440,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,12 +448,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="27.29071428571428" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="27.29071428571428" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -459,179 +463,94 @@
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>CPF</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Data Nascimento</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Endereço</t>
         </is>
       </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Senha</t>
+        </is>
+      </c>
     </row>
-    <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="1" t="n">
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>Ativado</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t>01912841223</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="inlineStr">
-        <is>
-          <t>Alefsander Ribeiro</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>23/10/1994</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="inlineStr">
-        <is>
-          <t>R. Escorpião, n° 11700 - Bairro: Ulisses Guimarães - Porto Velho/RO.</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>gAAAAABkGQIs4XrDiDGJ2xcI1ehSTjLWCVxshGwC8RmXjMG2oxpd0Y6Lu6yh3JutHhFVrJW5vbWMOE41WDR4BQSII-LxVgnz7w==</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>gAAAAABkGQIsLcyRxZpQHpcMJW3FXxT1kn6HWYYTNIeZihBdbmgaRfKKWYSYWpdEpQng4rIqOBrfvn1MnzGLKxBvaXrdrZ8PVcQri6hmyygUgP0H4t9-Sgc=</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>gAAAAABkGQIshVFHB9KYr8Ue8qyr2lfxl5ow9vlI6J3Gh1UVQVc-Vxgcvxs6ADFht0RWkSyiVI_MME_NvArs5ZYRSgX4H47avQ==</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>gAAAAABkGQIshYjB6GRppldInh63MYhcnGdAlX1U0XjLaGfBKtDNkS20mjUrKKd9tukMaOJoENDOHB561gfgtxJsyLp_C6FsGqKMlq7uu9Ksg5c6k_svutWxoL3uolzvXKNYK9KBdgXq6GeaNhExxXirt13IX4qHSj6w9v7t42Id1NnpTltW_I8=</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="1" t="n">
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Ativado</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>04240084245</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>Geissilaine Verônica</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t>19/107/1998</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>R. Maué, n° 4445 - Bairro: Socialista - Porto Velho/RO.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Ativado</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>123461365</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Alefsander Ribeiro</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>23/10/1994</t>
-        </is>
-      </c>
-      <c r="F4" s="4" t="inlineStr">
-        <is>
-          <t>R. Escorpião, n° 11700 - Bairro: Ulisses Guimarães - Porto Velho/RO.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Ativado</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>0191284122f1233</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>Alefsander Ribeiro</t>
-        </is>
-      </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t>23/10/1994</t>
-        </is>
-      </c>
-      <c r="F5" s="4" t="inlineStr">
-        <is>
-          <t>R. Escorpião, n° 11700 - Bairro: Ulisses Guimarães - Porto Velho/RO.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="19.5" customHeight="1">
-      <c r="A6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Ativado</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>123461365123</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>Alefsander Ribeiro</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t>23/10/1994</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="inlineStr">
-        <is>
-          <t>R. Escorpião, n° 11700 - Bairro: Ulisses Guimarães - Porto Velho/RO.</t>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>gAAAAABkGSX7ZFtt4vT2_b9jiGk-SvjrrCNCVGjncjftnvcnEzv_Qmq49-L-puG6SmlTkm9hatBHiOmEyfxwA0owS3kT2cUVTg==</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>gAAAAABkGSX7vS34tQ8JAg_snNny0v4n1kQMO-IstTjBWszuMyDglY9ixTf_CyyexTeyUUJq8FoldMXMjSCwtIdkhw9NYTABQfPAwBKRzjE0ukmpSqvhQps=</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>gAAAAABkGSX7Qmd8W_BGVvD1huwc-rcmUYtDJNsseBR5Iamj5wvRKE-RHBBOwjs_aZBkw1TJMJECU4faMQ4ONVzu6GXrTRwRNA==</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>gAAAAABkGSX7ReTmXIO7QKgYNwSJAvtF1F1SWADwS9o9pmjMTSlK6sOLeur_Y9R1-mLvxMvL9JsfILC5wrVRjEoJQH9FUNt7otBot587e0U46l_H_me0_Z-9QFuHaZ2mgokMvR-z6fVVBjUQEJ8o3GTwTjL9e3uNs4CrvlINVAk-io___Gnzbvw=</t>
         </is>
       </c>
     </row>

</xml_diff>